<commit_message>
1/19: to the script "replace-data", added rounding to 2 decimals, and changing date-format as well.
</commit_message>
<xml_diff>
--- a/replace-data.xlsx
+++ b/replace-data.xlsx
@@ -8,22 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prade\PycharmProjects\py-prj2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2BEB58-CFDF-491A-8F50-DE959A650422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC4907E-684C-46D3-A1A9-A36DAB4D5D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-53985" yWindow="2235" windowWidth="21600" windowHeight="12690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
-  <si>
-    <t>name of file</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>tag</t>
   </si>
@@ -31,9 +41,6 @@
     <t>trade1</t>
   </si>
   <si>
-    <t>actg-2026</t>
-  </si>
-  <si>
     <t>trade2</t>
   </si>
   <si>
@@ -59,6 +66,18 @@
   </si>
   <si>
     <t>trade10</t>
+  </si>
+  <si>
+    <t>actg-2024</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fileName</t>
   </si>
 </sst>
 </file>
@@ -88,7 +107,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -111,15 +130,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,102 +456,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>100.1234</v>
+      </c>
+      <c r="D2" s="3">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>101.9999</v>
+      </c>
+      <c r="D3" s="3">
+        <v>46024</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>110.1234</v>
+      </c>
+      <c r="D4" s="3">
+        <v>46025</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>120.3579</v>
+      </c>
+      <c r="D5" s="3">
+        <v>46026</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>120.1234</v>
+      </c>
+      <c r="D6" s="3">
+        <v>46027</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>130.3579</v>
+      </c>
+      <c r="D7" s="3">
+        <v>46028</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>130.1234</v>
+      </c>
+      <c r="D8" s="3">
+        <v>46029</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>140.3579</v>
+      </c>
+      <c r="D9" s="3">
+        <v>46030</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>140.1234</v>
+      </c>
+      <c r="D10" s="3">
+        <v>46031</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>150.3579</v>
+      </c>
+      <c r="D11" s="3">
+        <v>46032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>